<commit_message>
Write 2-step greedy function for sticky walls environment
</commit_message>
<xml_diff>
--- a/TransitionMatrixVariableLayout.xlsx
+++ b/TransitionMatrixVariableLayout.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="1D-9" sheetId="1" r:id="rId1"/>
+    <sheet name="1D-5" sheetId="2" r:id="rId2"/>
+    <sheet name="2D-5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="172">
   <si>
     <t>a</t>
   </si>
@@ -153,6 +154,384 @@
   </si>
   <si>
     <t>2 k w4 + m w5</t>
+  </si>
+  <si>
+    <t>w10</t>
+  </si>
+  <si>
+    <t>w11</t>
+  </si>
+  <si>
+    <t>w12</t>
+  </si>
+  <si>
+    <t>w13</t>
+  </si>
+  <si>
+    <t>w14</t>
+  </si>
+  <si>
+    <t>w15</t>
+  </si>
+  <si>
+    <t>w16</t>
+  </si>
+  <si>
+    <t>w17</t>
+  </si>
+  <si>
+    <t>w18</t>
+  </si>
+  <si>
+    <t>w19</t>
+  </si>
+  <si>
+    <t>w20</t>
+  </si>
+  <si>
+    <t>w21</t>
+  </si>
+  <si>
+    <t>w22</t>
+  </si>
+  <si>
+    <t>w23</t>
+  </si>
+  <si>
+    <t>w24</t>
+  </si>
+  <si>
+    <t>w25</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>x8</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>x10</t>
+  </si>
+  <si>
+    <t>x11</t>
+  </si>
+  <si>
+    <t>x12</t>
+  </si>
+  <si>
+    <t>x13</t>
+  </si>
+  <si>
+    <t>x14</t>
+  </si>
+  <si>
+    <t>x15</t>
+  </si>
+  <si>
+    <t>x16</t>
+  </si>
+  <si>
+    <t>x17</t>
+  </si>
+  <si>
+    <t>x18</t>
+  </si>
+  <si>
+    <t>x19</t>
+  </si>
+  <si>
+    <t>x20</t>
+  </si>
+  <si>
+    <t>x21</t>
+  </si>
+  <si>
+    <t>x22</t>
+  </si>
+  <si>
+    <t>x23</t>
+  </si>
+  <si>
+    <t>x24</t>
+  </si>
+  <si>
+    <t>x25</t>
+  </si>
+  <si>
+    <t>x26</t>
+  </si>
+  <si>
+    <t>x27</t>
+  </si>
+  <si>
+    <t>x28</t>
+  </si>
+  <si>
+    <t>x29</t>
+  </si>
+  <si>
+    <t>x30</t>
+  </si>
+  <si>
+    <t>x31</t>
+  </si>
+  <si>
+    <t>x32</t>
+  </si>
+  <si>
+    <t>x33</t>
+  </si>
+  <si>
+    <t>x34</t>
+  </si>
+  <si>
+    <t>x35</t>
+  </si>
+  <si>
+    <t>x36</t>
+  </si>
+  <si>
+    <t>x37</t>
+  </si>
+  <si>
+    <t>x38</t>
+  </si>
+  <si>
+    <t>x39</t>
+  </si>
+  <si>
+    <t>x40</t>
+  </si>
+  <si>
+    <t>x41</t>
+  </si>
+  <si>
+    <t>x42</t>
+  </si>
+  <si>
+    <t>x43</t>
+  </si>
+  <si>
+    <t>x44</t>
+  </si>
+  <si>
+    <t>x45</t>
+  </si>
+  <si>
+    <t>x46</t>
+  </si>
+  <si>
+    <t>x47</t>
+  </si>
+  <si>
+    <t>x48</t>
+  </si>
+  <si>
+    <t>x49</t>
+  </si>
+  <si>
+    <t>x50</t>
+  </si>
+  <si>
+    <t>x51</t>
+  </si>
+  <si>
+    <t>x52</t>
+  </si>
+  <si>
+    <t>x53</t>
+  </si>
+  <si>
+    <t>x54</t>
+  </si>
+  <si>
+    <t>x55</t>
+  </si>
+  <si>
+    <t>x56</t>
+  </si>
+  <si>
+    <t>x57</t>
+  </si>
+  <si>
+    <t>x58</t>
+  </si>
+  <si>
+    <t>x59</t>
+  </si>
+  <si>
+    <t>x60</t>
+  </si>
+  <si>
+    <t>x61</t>
+  </si>
+  <si>
+    <t>x62</t>
+  </si>
+  <si>
+    <t>x63</t>
+  </si>
+  <si>
+    <t>x64</t>
+  </si>
+  <si>
+    <t>x65</t>
+  </si>
+  <si>
+    <t>x66</t>
+  </si>
+  <si>
+    <t>x67</t>
+  </si>
+  <si>
+    <t>x68</t>
+  </si>
+  <si>
+    <t>x69</t>
+  </si>
+  <si>
+    <t>x70</t>
+  </si>
+  <si>
+    <t>x71</t>
+  </si>
+  <si>
+    <t>x72</t>
+  </si>
+  <si>
+    <t>x73</t>
+  </si>
+  <si>
+    <t>x74</t>
+  </si>
+  <si>
+    <t>x75</t>
+  </si>
+  <si>
+    <t>x76</t>
+  </si>
+  <si>
+    <t>x77</t>
+  </si>
+  <si>
+    <t>x78</t>
+  </si>
+  <si>
+    <t>x79</t>
+  </si>
+  <si>
+    <t>x80</t>
+  </si>
+  <si>
+    <t>x81</t>
+  </si>
+  <si>
+    <t>x82</t>
+  </si>
+  <si>
+    <t>x83</t>
+  </si>
+  <si>
+    <t>x84</t>
+  </si>
+  <si>
+    <t>x85</t>
+  </si>
+  <si>
+    <t>x86</t>
+  </si>
+  <si>
+    <t>x87</t>
+  </si>
+  <si>
+    <t>x88</t>
+  </si>
+  <si>
+    <t>x89</t>
+  </si>
+  <si>
+    <t>x90</t>
+  </si>
+  <si>
+    <t>x91</t>
+  </si>
+  <si>
+    <t>x92</t>
+  </si>
+  <si>
+    <t>x93</t>
+  </si>
+  <si>
+    <t>x94</t>
+  </si>
+  <si>
+    <t>x95</t>
+  </si>
+  <si>
+    <t>x96</t>
+  </si>
+  <si>
+    <t>x97</t>
+  </si>
+  <si>
+    <t>x98</t>
+  </si>
+  <si>
+    <t>x99</t>
+  </si>
+  <si>
+    <t>x100</t>
+  </si>
+  <si>
+    <t>x101</t>
+  </si>
+  <si>
+    <t>x102</t>
+  </si>
+  <si>
+    <t>x103</t>
+  </si>
+  <si>
+    <t>x104</t>
+  </si>
+  <si>
+    <t>x105</t>
+  </si>
+  <si>
+    <t>x1 w1 + x4 w2 + x19 w6</t>
+  </si>
+  <si>
+    <t>x2 w1 + x5 w2 + x8 w3 + x23 w7</t>
+  </si>
+  <si>
+    <t>x6 w2 + x9 w3 + x12 w4 + x28 w8</t>
+  </si>
+  <si>
+    <t>x10 w3 + x13 w4 + x16 w5 + x33 w9</t>
+  </si>
+  <si>
+    <t>x14 w4 + x17 w5 + x38 w10</t>
   </si>
 </sst>
 </file>
@@ -176,12 +555,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,12 +581,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1550,7 +1938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1882,4 +2272,2809 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:EF26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="39" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="129" width="4" bestFit="1" customWidth="1"/>
+    <col min="130" max="135" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CH2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CL2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="CN2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="CR2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="CS2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CT2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="CU2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="CV2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="CW2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="CX2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="CY2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DA2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="DB2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="DE2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="DF2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="DG2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DH2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="DI2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="DJ2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="DK2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="DL2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DM2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="DO2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="DP2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="DQ2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="DR2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="DS2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="DT2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DU2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="DV2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="DW2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="DX2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="DY2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="DZ2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="EA2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EB2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="ED2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="EE2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED3" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF3" s="1"/>
+    </row>
+    <row r="4" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED4" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED5" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED6" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED7" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>11</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>16</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>12</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>17</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>13</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>18</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>9</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>14</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>19</v>
+      </c>
+      <c r="AG15" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>20</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>